<commit_message>
Prepare time sheet, add formatting
</commit_message>
<xml_diff>
--- a/InetApp-Sprint11-tasks.xlsx
+++ b/InetApp-Sprint11-tasks.xlsx
@@ -2368,15 +2368,16 @@
   <dimension ref="A2:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
-    <col min="3" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="20" width="4" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -2443,15 +2444,15 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP($A3, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Organize the meeting with Harman Generic Browser responsibles</v>
-      </c>
-      <c r="C3" s="8" t="str">
+        <v>TRS: Revise complexity, revise API calls with focus to CRS</v>
+      </c>
+      <c r="C3" s="8">
         <f>VLOOKUP($A3, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1555</v>
+        <v>0</v>
       </c>
       <c r="D3" s="8" t="str">
         <f>VLOOKUP($A3, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2460,15 +2461,15 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP($A4, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Get application platform documented / get documentation</v>
-      </c>
-      <c r="C4" s="8" t="str">
+        <v>Get Application Platform documented</v>
+      </c>
+      <c r="C4" s="8">
         <f>VLOOKUP($A4, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1514</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>VLOOKUP($A4, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2477,15 +2478,15 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP($A5, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>TRS/CRS - remove links to Procom</v>
-      </c>
-      <c r="C5" s="8" t="str">
+        <v>HDD Document: complete deployment sec, process review notes.</v>
+      </c>
+      <c r="C5" s="8">
         <f>VLOOKUP($A5, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1513</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8" t="str">
         <f>VLOOKUP($A5, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2494,32 +2495,32 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP($A6, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Update TRS information for audio formats</v>
-      </c>
-      <c r="C6" s="8" t="str">
+        <v>Get Harman pres ctrl of Browser , interface understood.</v>
+      </c>
+      <c r="C6" s="8">
         <f>VLOOKUP($A6, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1513</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8" t="str">
         <f>VLOOKUP($A6, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
+        <v>Zolotykh Vladimir</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP($A7, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>HTML5 feature support for Browser</v>
-      </c>
-      <c r="C7" s="8" t="str">
+        <v>Coyote: update TRS and investigate, document test needs.</v>
+      </c>
+      <c r="C7" s="8">
         <f>VLOOKUP($A7, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1555</v>
+        <v>0</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>VLOOKUP($A7, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2528,53 +2529,53 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP($A8, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Coyote - add test needs to TRS</v>
-      </c>
-      <c r="C8" s="8" t="str">
+        <v>eStore: update TRS and investigate , document test needs.</v>
+      </c>
+      <c r="C8" s="8">
         <f>VLOOKUP($A8, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1556</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8" t="str">
         <f>VLOOKUP($A8, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
+        <v>Zolotykh Vladimir</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP($A9, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Estore - add test needs to TRS</v>
+        <v>TRS/CRS - remove links to Procom</v>
       </c>
       <c r="C9" s="8" t="str">
         <f>VLOOKUP($A9, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1557</v>
+        <v>HTOYOTA-1513</v>
       </c>
       <c r="D9" s="8" t="str">
         <f>VLOOKUP($A9, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
+        <v>Zolotykh Vladimir</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP($A10, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Application platform study</v>
+        <v>Update TRS information for audio formats</v>
       </c>
       <c r="C10" s="8" t="str">
         <f>VLOOKUP($A10, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1514</v>
+        <v>HTOYOTA-1513</v>
       </c>
       <c r="D10" s="8" t="str">
         <f>VLOOKUP($A10, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Zolotykh Vladimir</v>
+        <v>Dan Sava</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2613,15 +2614,15 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP($A13, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Extend HDD with Browser description</v>
+        <v>CRS editions, rephrasing and making the statesments clearer and more precise.</v>
       </c>
       <c r="C13" s="8" t="str">
         <f>VLOOKUP($A13, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1515</v>
+        <v>HTOYOTA-1513</v>
       </c>
       <c r="D13" s="8" t="str">
         <f>VLOOKUP($A13, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2630,15 +2631,15 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP($A14, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>analyse Presentation controller document from Browser</v>
+        <v>Conduct TRS review with Mr. Lanckman</v>
       </c>
       <c r="C14" s="8" t="str">
         <f>VLOOKUP($A14, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1555</v>
+        <v>HTOYOTA-1513</v>
       </c>
       <c r="D14" s="8" t="str">
         <f>VLOOKUP($A14, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2647,45 +2648,42 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP($A15, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>eStore: Check if all interactions with application platform/other parts of the system are available in the application platform specification</v>
+        <v>Add non-functional requirements (TRS)</v>
       </c>
       <c r="C15" s="8" t="str">
         <f>VLOOKUP($A15, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1557</v>
+        <v>HTOYOTA-1513</v>
       </c>
       <c r="D15" s="8" t="str">
         <f>VLOOKUP($A15, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
+        <v>Roman Nikitin</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B16" t="str">
-        <f>VLOOKUP($A16, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>CRS editions, rephrasing and making the statesments clearer and more precise.</v>
+        <f>VLOOKUP(A16, general_report!A31:L59, 2, FALSE)</f>
+        <v>Update initial chapters of TRS , DOORS</v>
       </c>
       <c r="C16" s="8" t="str">
         <f>VLOOKUP($A16, general_report!$A$3:$L$31, 3, FALSE)</f>
         <v>HTOYOTA-1513</v>
       </c>
-      <c r="D16" s="8" t="str">
-        <f>VLOOKUP($A16, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
-      </c>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP($A17, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Resolving IT related issues ( accounts, rights, access, etc.)</v>
+        <v>Get application platform documented / get documentation</v>
       </c>
       <c r="C17" s="8" t="str">
         <f>VLOOKUP($A17, general_report!$A$3:$L$31, 3, FALSE)</f>
@@ -2698,32 +2696,32 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP($A18, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Update TRS for Coyote to include Coyote Screens - Settings</v>
+        <v>Application platform study</v>
       </c>
       <c r="C18" s="8" t="str">
         <f>VLOOKUP($A18, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1556</v>
+        <v>HTOYOTA-1514</v>
       </c>
       <c r="D18" s="8" t="str">
         <f>VLOOKUP($A18, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Dan Sava</v>
+        <v>Zolotykh Vladimir</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP($A19, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>TRS: Revise complexity, revise API calls with focus to CRS</v>
-      </c>
-      <c r="C19" s="8">
+        <v>Resolving IT related issues ( accounts, rights, access, etc.)</v>
+      </c>
+      <c r="C19" s="8" t="str">
         <f>VLOOKUP($A19, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1514</v>
       </c>
       <c r="D19" s="8" t="str">
         <f>VLOOKUP($A19, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2732,49 +2730,49 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP($A20, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Get Application Platform documented</v>
-      </c>
-      <c r="C20" s="8">
+        <v>Extend HDD with Browser description</v>
+      </c>
+      <c r="C20" s="8" t="str">
         <f>VLOOKUP($A20, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1515</v>
       </c>
       <c r="D20" s="8" t="str">
         <f>VLOOKUP($A20, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Zolotykh Vladimir</v>
+        <v>Dan Sava</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP($A21, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>HDD Document: complete deployment sec, process review notes.</v>
-      </c>
-      <c r="C21" s="8">
+        <v>Process HDD review notes by Mr. Lanckman and make necessary corrections in the HDD</v>
+      </c>
+      <c r="C21" s="8" t="str">
         <f>VLOOKUP($A21, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1515</v>
       </c>
       <c r="D21" s="8" t="str">
         <f>VLOOKUP($A21, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Zolotykh Vladimir</v>
+        <v>Roman Nikitin</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP($A22, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Get Harman pres ctrl of Browser , interface understood.</v>
-      </c>
-      <c r="C22" s="8">
+        <v>Conduct the HDD review with Mr. Lanckman</v>
+      </c>
+      <c r="C22" s="8" t="str">
         <f>VLOOKUP($A22, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1515</v>
       </c>
       <c r="D22" s="8" t="str">
         <f>VLOOKUP($A22, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2783,32 +2781,32 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP($A23, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Coyote: update TRS and investigate, document test needs.</v>
-      </c>
-      <c r="C23" s="8">
+        <v>Extend / update HDD with Application framework description</v>
+      </c>
+      <c r="C23" s="8" t="str">
         <f>VLOOKUP($A23, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1515</v>
       </c>
       <c r="D23" s="8" t="str">
         <f>VLOOKUP($A23, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Zolotykh Vladimir</v>
+        <v>Dan Sava</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP($A24, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>eStore: update TRS and investigate , document test needs.</v>
-      </c>
-      <c r="C24" s="8">
+        <v>Finalize Deployment section of the HDD</v>
+      </c>
+      <c r="C24" s="8" t="str">
         <f>VLOOKUP($A24, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>0</v>
+        <v>HTOYOTA-1515</v>
       </c>
       <c r="D24" s="8" t="str">
         <f>VLOOKUP($A24, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2817,32 +2815,32 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP($A25, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Process HDD review notes by Mr. Lanckman and make necessary corrections in the HDD</v>
+        <v>Organize the meeting with Harman Generic Browser responsibles</v>
       </c>
       <c r="C25" s="8" t="str">
         <f>VLOOKUP($A25, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1515</v>
+        <v>HTOYOTA-1555</v>
       </c>
       <c r="D25" s="8" t="str">
         <f>VLOOKUP($A25, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Roman Nikitin</v>
+        <v>Zolotykh Vladimir</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP($A26, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Conduct the HDD review with Mr. Lanckman</v>
+        <v>HTML5 feature support for Browser</v>
       </c>
       <c r="C26" s="8" t="str">
         <f>VLOOKUP($A26, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1515</v>
+        <v>HTOYOTA-1555</v>
       </c>
       <c r="D26" s="8" t="str">
         <f>VLOOKUP($A26, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2851,15 +2849,15 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP($A27, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Conduct TRS review with Mr. Lanckman</v>
+        <v>analyse Presentation controller document from Browser</v>
       </c>
       <c r="C27" s="8" t="str">
         <f>VLOOKUP($A27, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1513</v>
+        <v>HTOYOTA-1555</v>
       </c>
       <c r="D27" s="8" t="str">
         <f>VLOOKUP($A27, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2868,32 +2866,32 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP($A28, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Add non-functional requirements (TRS)</v>
+        <v>Coyote - add test needs to TRS</v>
       </c>
       <c r="C28" s="8" t="str">
         <f>VLOOKUP($A28, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1513</v>
+        <v>HTOYOTA-1556</v>
       </c>
       <c r="D28" s="8" t="str">
         <f>VLOOKUP($A28, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Roman Nikitin</v>
+        <v>Dan Sava</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP($A29, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Extend / update HDD with Application framework description</v>
+        <v>Update TRS for Coyote to include Coyote Screens - Settings</v>
       </c>
       <c r="C29" s="8" t="str">
         <f>VLOOKUP($A29, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1515</v>
+        <v>HTOYOTA-1556</v>
       </c>
       <c r="D29" s="8" t="str">
         <f>VLOOKUP($A29, general_report!$A$3:$L$31, 5, FALSE)</f>
@@ -2902,67 +2900,74 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP($A30, general_report!$A$3:$L$31, 2, FALSE)</f>
-        <v>Finalize Deployment section of the HDD</v>
+        <v>Estore - add test needs to TRS</v>
       </c>
       <c r="C30" s="8" t="str">
         <f>VLOOKUP($A30, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1515</v>
+        <v>HTOYOTA-1557</v>
       </c>
       <c r="D30" s="8" t="str">
         <f>VLOOKUP($A30, general_report!$A$3:$L$31, 5, FALSE)</f>
-        <v>Zolotykh Vladimir</v>
+        <v>Dan Sava</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B31" t="str">
-        <f>VLOOKUP(A31, general_report!A31:L59, 2, FALSE)</f>
-        <v>Update initial chapters of TRS , DOORS</v>
+        <f>VLOOKUP($A31, general_report!$A$3:$L$31, 2, FALSE)</f>
+        <v>eStore: Check if all interactions with application platform/other parts of the system are available in the application platform specification</v>
       </c>
       <c r="C31" s="8" t="str">
         <f>VLOOKUP($A31, general_report!$A$3:$L$31, 3, FALSE)</f>
-        <v>HTOYOTA-1513</v>
-      </c>
-      <c r="D31" s="8"/>
+        <v>HTOYOTA-1557</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f>VLOOKUP($A31, general_report!$A$3:$L$31, 5, FALSE)</f>
+        <v>Dan Sava</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T31"/>
+  <autoFilter ref="A2:T31">
+    <sortState ref="A3:T31">
+      <sortCondition ref="C2:C31"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="A27" r:id="rId1" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1588"/>
-    <hyperlink ref="A26" r:id="rId2" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1587"/>
-    <hyperlink ref="A25" r:id="rId3" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1586"/>
-    <hyperlink ref="A24" r:id="rId4" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1557"/>
-    <hyperlink ref="A23" r:id="rId5" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1556"/>
-    <hyperlink ref="A22" r:id="rId6" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1555"/>
-    <hyperlink ref="A21" r:id="rId7" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1515"/>
-    <hyperlink ref="A20" r:id="rId8" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1514"/>
-    <hyperlink ref="A19" r:id="rId9" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1513"/>
-    <hyperlink ref="A18" r:id="rId10" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1509"/>
-    <hyperlink ref="A17" r:id="rId11" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1508"/>
-    <hyperlink ref="A16" r:id="rId12" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1507"/>
-    <hyperlink ref="A15" r:id="rId13" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1476"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1474"/>
-    <hyperlink ref="A13" r:id="rId15" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1473"/>
+    <hyperlink ref="A14" r:id="rId1" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1588"/>
+    <hyperlink ref="A22" r:id="rId2" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1587"/>
+    <hyperlink ref="A21" r:id="rId3" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1586"/>
+    <hyperlink ref="A8" r:id="rId4" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1557"/>
+    <hyperlink ref="A7" r:id="rId5" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1556"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1555"/>
+    <hyperlink ref="A5" r:id="rId7" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1515"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1514"/>
+    <hyperlink ref="A3" r:id="rId9" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1513"/>
+    <hyperlink ref="A29" r:id="rId10" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1509"/>
+    <hyperlink ref="A19" r:id="rId11" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1508"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1507"/>
+    <hyperlink ref="A31" r:id="rId13" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1476"/>
+    <hyperlink ref="A27" r:id="rId14" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1474"/>
+    <hyperlink ref="A20" r:id="rId15" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1473"/>
     <hyperlink ref="A12" r:id="rId16" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1471"/>
     <hyperlink ref="A11" r:id="rId17" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1403"/>
-    <hyperlink ref="A10" r:id="rId18" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1371"/>
-    <hyperlink ref="A9" r:id="rId19" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1290"/>
-    <hyperlink ref="A8" r:id="rId20" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1289"/>
-    <hyperlink ref="A7" r:id="rId21" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1288"/>
-    <hyperlink ref="A6" r:id="rId22" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1281"/>
-    <hyperlink ref="A5" r:id="rId23" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1143"/>
-    <hyperlink ref="A4" r:id="rId24" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1086"/>
-    <hyperlink ref="A3" r:id="rId25" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1085"/>
-    <hyperlink ref="A31" r:id="rId26" display="https://adc.luxoft.com/jira/browse/HTOYOTA-885"/>
-    <hyperlink ref="A30" r:id="rId27" display="https://adc.luxoft.com/jira/browse/HTOYOTA-861"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://adc.luxoft.com/jira/browse/HTOYOTA-748"/>
-    <hyperlink ref="A28" r:id="rId29" display="https://adc.luxoft.com/jira/browse/HTOYOTA-717"/>
+    <hyperlink ref="A18" r:id="rId18" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1371"/>
+    <hyperlink ref="A30" r:id="rId19" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1290"/>
+    <hyperlink ref="A28" r:id="rId20" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1289"/>
+    <hyperlink ref="A26" r:id="rId21" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1288"/>
+    <hyperlink ref="A10" r:id="rId22" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1281"/>
+    <hyperlink ref="A9" r:id="rId23" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1143"/>
+    <hyperlink ref="A17" r:id="rId24" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1086"/>
+    <hyperlink ref="A25" r:id="rId25" display="https://adc.luxoft.com/jira/browse/HTOYOTA-1085"/>
+    <hyperlink ref="A16" r:id="rId26" display="https://adc.luxoft.com/jira/browse/HTOYOTA-885"/>
+    <hyperlink ref="A24" r:id="rId27" display="https://adc.luxoft.com/jira/browse/HTOYOTA-861"/>
+    <hyperlink ref="A23" r:id="rId28" display="https://adc.luxoft.com/jira/browse/HTOYOTA-748"/>
+    <hyperlink ref="A15" r:id="rId29" display="https://adc.luxoft.com/jira/browse/HTOYOTA-717"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>